<commit_message>
Update RePORT_DEB_to_Tables_mapping.xlsx with revised data mapping specifications
</commit_message>
<xml_diff>
--- a/data/data_dictionary_and_mapping_specifications/RePORT_DEB_to_Tables_mapping.xlsx
+++ b/data/data_dictionary_and_mapping_specifications/RePORT_DEB_to_Tables_mapping.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sj1136/Documents/VSCode_files/gitRepo/Work/ChatBotRAG/data/data_dictionary_and_mapping_specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420BA64A-BC00-144B-8708-1526A883F501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCCF863-CDC9-754F-8909-BE5096AFE8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="25960" windowHeight="19000" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="25960" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="New Codelists" sheetId="1" r:id="rId1"/>
+    <sheet name="Codelists" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
     <sheet name="tblENROL" sheetId="3" r:id="rId3"/>
     <sheet name="tblHISTORY" sheetId="4" r:id="rId4"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5701" uniqueCount="2282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5702" uniqueCount="2282">
   <si>
     <t>Codelist</t>
   </si>
@@ -7657,7 +7657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -8053,6 +8053,9 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8306,8 +8309,8 @@
   </sheetPr>
   <dimension ref="A1:Z1160"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -44383,7 +44386,7 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -44776,7 +44779,7 @@
   </sheetPr>
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -47670,7 +47673,7 @@
   </sheetPr>
   <dimension ref="A1:AD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -49570,7 +49573,7 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -50315,7 +50318,7 @@
   </sheetPr>
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -53694,8 +53697,8 @@
   </sheetPr>
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -54505,7 +54508,7 @@
       <c r="I18" s="79" t="s">
         <v>1007</v>
       </c>
-      <c r="J18" s="79" t="s">
+      <c r="J18" s="169" t="s">
         <v>1068</v>
       </c>
       <c r="K18" s="79"/>
@@ -55546,8 +55549,8 @@
   </sheetPr>
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -57394,7 +57397,7 @@
   <dimension ref="A1:AD1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -57453,7 +57456,9 @@
       <c r="P1" s="58" t="s">
         <v>1001</v>
       </c>
-      <c r="Q1" s="24"/>
+      <c r="Q1" s="166" t="s">
+        <v>2280</v>
+      </c>
       <c r="R1" s="24"/>
       <c r="S1" s="24"/>
       <c r="T1" s="24"/>
@@ -62109,7 +62114,7 @@
   </sheetPr>
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="S61" sqref="S61"/>
     </sheetView>
   </sheetViews>
@@ -64747,7 +64752,7 @@
   </sheetPr>
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enhance logging for Codelists sheet in load_dictionary.py: Added note for distinct tables in the sheet.
</commit_message>
<xml_diff>
--- a/data/data_dictionary_and_mapping_specifications/RePORT_DEB_to_Tables_mapping.xlsx
+++ b/data/data_dictionary_and_mapping_specifications/RePORT_DEB_to_Tables_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sj1136/Documents/VSCode_files/gitRepo/Work/ChatBotRAG/data/data_dictionary_and_mapping_specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCCF863-CDC9-754F-8909-BE5096AFE8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24270CA-4F3D-C043-9BBD-9201F72D0F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="25960" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8309,8 +8309,8 @@
   </sheetPr>
   <dimension ref="A1:Z1160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8342,7 +8342,6 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -8380,7 +8379,6 @@
       <c r="G2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -8418,7 +8416,6 @@
       <c r="G3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -8456,7 +8453,6 @@
       <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -8494,7 +8490,6 @@
       <c r="G5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -8532,7 +8527,6 @@
       <c r="G6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -8570,7 +8564,6 @@
       <c r="G7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -8608,7 +8601,6 @@
       <c r="G8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -8646,7 +8638,6 @@
       <c r="G9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -8684,7 +8675,6 @@
       <c r="G10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -8722,7 +8712,6 @@
       <c r="G11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -8760,7 +8749,6 @@
       <c r="G12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -8798,7 +8786,6 @@
       <c r="G13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -8836,7 +8823,6 @@
       <c r="G14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -8874,7 +8860,6 @@
       <c r="G15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -8912,7 +8897,6 @@
       <c r="G16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -8952,7 +8936,6 @@
       <c r="G17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -8990,7 +8973,6 @@
       <c r="G18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -9030,7 +9012,6 @@
       <c r="G19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -9068,7 +9049,6 @@
       <c r="G20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -9171,7 +9151,6 @@
       <c r="F23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -9207,7 +9186,6 @@
       <c r="F24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -9243,7 +9221,6 @@
       <c r="F25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -9277,7 +9254,6 @@
       <c r="D26" s="9"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -9313,7 +9289,6 @@
       <c r="F27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -9349,7 +9324,6 @@
       <c r="F28" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>

</xml_diff>